<commit_message>
Changed propery to Real estate
</commit_message>
<xml_diff>
--- a/Peer_companies/Ticker-list.xlsx
+++ b/Peer_companies/Ticker-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odin Mjølsnes\Documents\myrepo2\Peer_companies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matilde\Documents\Master\myrepo\Peer_companies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237DD193-09A9-4175-8E11-8E44702A2CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB27FED-C4CA-4624-B6FB-80610E387D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CD468C8E-59AE-4EB8-BBB3-7335E9F5A281}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD468C8E-59AE-4EB8-BBB3-7335E9F5A281}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1545,9 +1545,6 @@
     <t>Baltic Sea Properties</t>
   </si>
   <si>
-    <t>Property</t>
-  </si>
-  <si>
     <t>Eiendom</t>
   </si>
   <si>
@@ -1666,6 +1663,9 @@
   </si>
   <si>
     <t>Tysnes Sparebank</t>
+  </si>
+  <si>
+    <t>Real_estate</t>
   </si>
 </sst>
 </file>
@@ -2041,17 +2041,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4578A8B3-0529-474E-BC66-78BDA5434747}">
   <dimension ref="A1:D265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D265"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="G231" sqref="G231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>263</v>
       </c>
@@ -2065,7 +2067,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2079,7 +2081,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2093,7 +2095,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2107,7 +2109,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2121,7 +2123,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2135,7 +2137,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2163,7 +2165,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2177,7 +2179,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2191,7 +2193,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2205,7 +2207,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2219,7 +2221,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -2233,7 +2235,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -2247,7 +2249,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2261,7 +2263,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2275,7 +2277,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2289,7 +2291,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -2303,7 +2305,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2317,7 +2319,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -2331,7 +2333,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -2345,7 +2347,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -2359,7 +2361,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -2387,7 +2389,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -2415,7 +2417,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -2429,7 +2431,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -2443,7 +2445,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>92</v>
       </c>
@@ -2457,7 +2459,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -2471,7 +2473,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -2485,7 +2487,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -2499,7 +2501,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>122</v>
       </c>
@@ -2513,7 +2515,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>129</v>
       </c>
@@ -2527,7 +2529,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>149</v>
       </c>
@@ -2541,7 +2543,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>142</v>
       </c>
@@ -2555,7 +2557,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -2569,7 +2571,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -2583,7 +2585,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -2597,7 +2599,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -2611,7 +2613,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>159</v>
       </c>
@@ -2625,7 +2627,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>162</v>
       </c>
@@ -2639,7 +2641,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>160</v>
       </c>
@@ -2653,7 +2655,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>169</v>
       </c>
@@ -2667,7 +2669,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>182</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>177</v>
       </c>
@@ -2695,7 +2697,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>171</v>
       </c>
@@ -2709,7 +2711,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>174</v>
       </c>
@@ -2723,7 +2725,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -2737,7 +2739,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>183</v>
       </c>
@@ -2751,7 +2753,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>186</v>
       </c>
@@ -2765,7 +2767,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>187</v>
       </c>
@@ -2779,7 +2781,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>210</v>
       </c>
@@ -2793,7 +2795,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -2807,7 +2809,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>209</v>
       </c>
@@ -2821,7 +2823,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>211</v>
       </c>
@@ -2835,7 +2837,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>213</v>
       </c>
@@ -2849,7 +2851,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>218</v>
       </c>
@@ -2863,7 +2865,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>231</v>
       </c>
@@ -2877,7 +2879,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>238</v>
       </c>
@@ -2891,7 +2893,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>261</v>
       </c>
@@ -2905,7 +2907,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -2919,7 +2921,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -2933,7 +2935,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>45</v>
       </c>
@@ -2947,7 +2949,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -2961,7 +2963,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -2975,7 +2977,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -2989,7 +2991,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>145</v>
       </c>
@@ -3003,7 +3005,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -3017,7 +3019,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>153</v>
       </c>
@@ -3031,7 +3033,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>206</v>
       </c>
@@ -3045,7 +3047,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>258</v>
       </c>
@@ -3059,7 +3061,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2020</v>
       </c>
@@ -3073,7 +3075,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -3087,7 +3089,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -3101,7 +3103,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -3115,7 +3117,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -3129,7 +3131,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -3143,7 +3145,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -3157,7 +3159,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -3171,7 +3173,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>23</v>
       </c>
@@ -3185,7 +3187,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>40</v>
       </c>
@@ -3199,7 +3201,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -3213,7 +3215,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>43</v>
       </c>
@@ -3227,7 +3229,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>67</v>
       </c>
@@ -3241,7 +3243,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>74</v>
       </c>
@@ -3255,7 +3257,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>190</v>
       </c>
@@ -3269,7 +3271,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -3283,7 +3285,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -3297,7 +3299,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -3311,7 +3313,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>106</v>
       </c>
@@ -3339,7 +3341,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>109</v>
       </c>
@@ -3353,7 +3355,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>113</v>
       </c>
@@ -3367,7 +3369,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>127</v>
       </c>
@@ -3381,7 +3383,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>130</v>
       </c>
@@ -3395,7 +3397,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>140</v>
       </c>
@@ -3409,7 +3411,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>136</v>
       </c>
@@ -3423,7 +3425,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>133</v>
       </c>
@@ -3437,7 +3439,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>151</v>
       </c>
@@ -3451,7 +3453,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>154</v>
       </c>
@@ -3465,7 +3467,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>157</v>
       </c>
@@ -3479,7 +3481,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>158</v>
       </c>
@@ -3493,7 +3495,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>161</v>
       </c>
@@ -3507,7 +3509,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>172</v>
       </c>
@@ -3521,7 +3523,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>185</v>
       </c>
@@ -3535,7 +3537,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>199</v>
       </c>
@@ -3549,7 +3551,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>226</v>
       </c>
@@ -3563,7 +3565,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>215</v>
       </c>
@@ -3577,7 +3579,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>236</v>
       </c>
@@ -3591,7 +3593,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>241</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>243</v>
       </c>
@@ -3619,7 +3621,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>248</v>
       </c>
@@ -3633,7 +3635,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>250</v>
       </c>
@@ -3647,7 +3649,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>252</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>255</v>
       </c>
@@ -3675,7 +3677,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>256</v>
       </c>
@@ -3689,7 +3691,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>253</v>
       </c>
@@ -3703,7 +3705,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>259</v>
       </c>
@@ -3717,7 +3719,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>260</v>
       </c>
@@ -3731,7 +3733,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -3759,7 +3761,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>22</v>
       </c>
@@ -3773,7 +3775,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>24</v>
       </c>
@@ -3787,7 +3789,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>30</v>
       </c>
@@ -3801,7 +3803,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>37</v>
       </c>
@@ -3815,7 +3817,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>85</v>
       </c>
@@ -3829,7 +3831,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>98</v>
       </c>
@@ -3843,7 +3845,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>118</v>
       </c>
@@ -3857,7 +3859,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>126</v>
       </c>
@@ -3871,7 +3873,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>134</v>
       </c>
@@ -3885,7 +3887,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>152</v>
       </c>
@@ -3899,7 +3901,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>164</v>
       </c>
@@ -3913,7 +3915,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>196</v>
       </c>
@@ -3927,7 +3929,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>197</v>
       </c>
@@ -3941,7 +3943,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>198</v>
       </c>
@@ -3955,7 +3957,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>49</v>
       </c>
@@ -3969,7 +3971,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>70</v>
       </c>
@@ -3983,7 +3985,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>80</v>
       </c>
@@ -3997,7 +3999,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>86</v>
       </c>
@@ -4011,7 +4013,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>110</v>
       </c>
@@ -4025,7 +4027,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>112</v>
       </c>
@@ -4039,7 +4041,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>191</v>
       </c>
@@ -4053,7 +4055,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>200</v>
       </c>
@@ -4067,7 +4069,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>257</v>
       </c>
@@ -4081,7 +4083,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>35</v>
       </c>
@@ -4095,7 +4097,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>42</v>
       </c>
@@ -4109,7 +4111,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>53</v>
       </c>
@@ -4123,7 +4125,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>55</v>
       </c>
@@ -4137,7 +4139,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>57</v>
       </c>
@@ -4151,7 +4153,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>72</v>
       </c>
@@ -4165,7 +4167,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>78</v>
       </c>
@@ -4179,7 +4181,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>89</v>
       </c>
@@ -4193,7 +4195,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>117</v>
       </c>
@@ -4207,7 +4209,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>120</v>
       </c>
@@ -4221,7 +4223,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>135</v>
       </c>
@@ -4235,7 +4237,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>131</v>
       </c>
@@ -4249,7 +4251,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>155</v>
       </c>
@@ -4263,7 +4265,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>168</v>
       </c>
@@ -4277,7 +4279,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>173</v>
       </c>
@@ -4291,7 +4293,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>219</v>
       </c>
@@ -4305,7 +4307,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>244</v>
       </c>
@@ -4319,7 +4321,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>246</v>
       </c>
@@ -4333,7 +4335,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>247</v>
       </c>
@@ -4347,7 +4349,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>249</v>
       </c>
@@ -4361,7 +4363,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>25</v>
       </c>
@@ -4375,7 +4377,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>12</v>
       </c>
@@ -4389,7 +4391,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>33</v>
       </c>
@@ -4403,7 +4405,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>36</v>
       </c>
@@ -4417,7 +4419,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>47</v>
       </c>
@@ -4431,7 +4433,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>58</v>
       </c>
@@ -4445,7 +4447,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>81</v>
       </c>
@@ -4459,7 +4461,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>100</v>
       </c>
@@ -4473,7 +4475,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>101</v>
       </c>
@@ -4487,7 +4489,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>102</v>
       </c>
@@ -4501,7 +4503,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>114</v>
       </c>
@@ -4515,7 +4517,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>143</v>
       </c>
@@ -4529,7 +4531,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>167</v>
       </c>
@@ -4543,7 +4545,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -4557,7 +4559,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>195</v>
       </c>
@@ -4571,7 +4573,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>201</v>
       </c>
@@ -4585,7 +4587,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>225</v>
       </c>
@@ -4599,7 +4601,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>228</v>
       </c>
@@ -4613,7 +4615,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>251</v>
       </c>
@@ -4627,7 +4629,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>26</v>
       </c>
@@ -4641,7 +4643,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>27</v>
       </c>
@@ -4655,7 +4657,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>34</v>
       </c>
@@ -4669,7 +4671,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>46</v>
       </c>
@@ -4683,7 +4685,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>56</v>
       </c>
@@ -4697,7 +4699,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>65</v>
       </c>
@@ -4711,7 +4713,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>97</v>
       </c>
@@ -4725,7 +4727,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>99</v>
       </c>
@@ -4739,7 +4741,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>104</v>
       </c>
@@ -4753,7 +4755,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>111</v>
       </c>
@@ -4767,7 +4769,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>128</v>
       </c>
@@ -4781,7 +4783,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>124</v>
       </c>
@@ -4795,7 +4797,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>132</v>
       </c>
@@ -4809,7 +4811,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>137</v>
       </c>
@@ -4823,7 +4825,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>148</v>
       </c>
@@ -4837,7 +4839,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>141</v>
       </c>
@@ -4851,7 +4853,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>170</v>
       </c>
@@ -4865,7 +4867,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>175</v>
       </c>
@@ -4879,7 +4881,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>184</v>
       </c>
@@ -4893,7 +4895,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>188</v>
       </c>
@@ -4907,7 +4909,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>212</v>
       </c>
@@ -4921,7 +4923,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>230</v>
       </c>
@@ -4935,7 +4937,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>235</v>
       </c>
@@ -4949,7 +4951,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>239</v>
       </c>
@@ -4963,7 +4965,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>240</v>
       </c>
@@ -4977,7 +4979,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>254</v>
       </c>
@@ -4991,7 +4993,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>262</v>
       </c>
@@ -5005,7 +5007,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>73</v>
       </c>
@@ -5019,7 +5021,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>3</v>
       </c>
@@ -5033,7 +5035,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>96</v>
       </c>
@@ -5047,7 +5049,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>108</v>
       </c>
@@ -5061,7 +5063,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>116</v>
       </c>
@@ -5075,7 +5077,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>165</v>
       </c>
@@ -5089,7 +5091,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>176</v>
       </c>
@@ -5103,7 +5105,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>178</v>
       </c>
@@ -5117,7 +5119,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>207</v>
       </c>
@@ -5131,7 +5133,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>208</v>
       </c>
@@ -5145,7 +5147,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>237</v>
       </c>
@@ -5159,7 +5161,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>5</v>
       </c>
@@ -5173,7 +5175,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>54</v>
       </c>
@@ -5187,7 +5189,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>61</v>
       </c>
@@ -5201,7 +5203,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>75</v>
       </c>
@@ -5215,7 +5217,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>227</v>
       </c>
@@ -5229,7 +5231,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>38</v>
       </c>
@@ -5237,528 +5239,528 @@
         <v>502</v>
       </c>
       <c r="C228" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D228" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D228" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>68</v>
       </c>
       <c r="B229" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C229" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D229" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D229" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>150</v>
       </c>
       <c r="B230" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C230" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D230" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D230" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>163</v>
       </c>
       <c r="B231" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C231" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D231" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D231" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>179</v>
       </c>
       <c r="B232" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C232" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D232" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D232" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>192</v>
       </c>
       <c r="B233" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C233" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D233" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D233" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>202</v>
       </c>
       <c r="B234" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C234" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D234" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D234" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>221</v>
       </c>
       <c r="B235" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C235" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D235" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D235" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>229</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="C236" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D236" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="D236" s="3" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="237" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>0</v>
       </c>
       <c r="B237" t="s">
+        <v>512</v>
+      </c>
+      <c r="C237" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C237" s="1" t="s">
+      <c r="D237" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D237" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="238" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>29</v>
       </c>
       <c r="B238" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C238" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D238" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D238" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="239" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>84</v>
       </c>
       <c r="B239" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C239" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D239" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D239" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="240" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>90</v>
       </c>
       <c r="B240" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C240" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D240" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D240" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="241" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>93</v>
       </c>
       <c r="B241" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C241" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D241" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D241" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="242" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>105</v>
       </c>
       <c r="B242" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C242" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D242" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D242" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="243" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>119</v>
       </c>
       <c r="B243" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C243" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D243" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D243" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="244" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>121</v>
       </c>
       <c r="B244" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C244" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D244" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D244" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="245" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>139</v>
       </c>
       <c r="B245" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C245" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D245" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D245" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="246" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>193</v>
       </c>
       <c r="B246" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C246" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D246" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D246" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="247" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>194</v>
       </c>
       <c r="B247" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C247" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D247" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D247" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="248" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>214</v>
       </c>
       <c r="B248" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C248" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D248" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D248" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="249" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>220</v>
       </c>
       <c r="B249" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C249" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D249" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D249" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="250" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>204</v>
       </c>
       <c r="B250" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C250" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D250" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D250" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="251" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>146</v>
       </c>
       <c r="B251" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C251" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D251" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D251" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="252" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>216</v>
       </c>
       <c r="B252" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C252" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D252" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D252" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="253" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>189</v>
       </c>
       <c r="B253" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C253" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D253" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D253" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="254" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>123</v>
       </c>
       <c r="B254" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C254" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D254" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D254" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="255" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>217</v>
       </c>
       <c r="B255" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C255" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D255" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D255" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="256" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>224</v>
       </c>
       <c r="B256" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C256" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D256" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D256" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="257" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>125</v>
       </c>
       <c r="B257" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C257" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D257" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D257" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="258" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>222</v>
       </c>
       <c r="B258" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C258" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D258" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D258" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="259" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>203</v>
       </c>
       <c r="B259" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C259" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D259" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D259" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="260" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>234</v>
       </c>
       <c r="B260" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C260" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D260" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D260" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="261" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>223</v>
       </c>
       <c r="B261" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C261" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D261" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D261" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="262" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="262" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>232</v>
       </c>
       <c r="B262" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C262" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D262" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D262" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="263" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>233</v>
       </c>
       <c r="B263" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C263" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D263" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D263" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="264" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>242</v>
       </c>
       <c r="B264" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C264" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D264" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D264" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="265" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>245</v>
       </c>
       <c r="B265" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C265" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D265" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="D265" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>